<commit_message>
Demo completa y funcional
Busqueda de informacion de usuarios concretos todo ok
</commit_message>
<xml_diff>
--- a/exports/instagram_joanpradells.xlsx
+++ b/exports/instagram_joanpradells.xlsx
@@ -495,10 +495,10 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>755332</v>
+        <v>755238</v>
       </c>
       <c r="G2" t="n">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -507,7 +507,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>no_encontrado</t>
+          <t>no_email</t>
         </is>
       </c>
     </row>

</xml_diff>